<commit_message>
Replace project with updated version
</commit_message>
<xml_diff>
--- a/next_week_weights_estimate_app.xlsx
+++ b/next_week_weights_estimate_app.xlsx
@@ -469,19 +469,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.999999996554006</v>
+        <v>0.9999999812490273</v>
       </c>
       <c r="C2" t="n">
-        <v>7.71714358019754e-10</v>
+        <v>3.055467619578929e-09</v>
       </c>
       <c r="D2" t="n">
-        <v>1.028879008512616e-09</v>
+        <v>2.787152827383198e-09</v>
       </c>
       <c r="E2" t="n">
-        <v>1.645425333346985e-09</v>
+        <v>1.290841546880258e-08</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>46038</v>
+        <v>46045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>